<commit_message>
fixed issues with parsing of Instance sheet for values which are different than strings
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/source-to-solution-mapping-rules.xlsx
+++ b/cognite/neat/examples/rules/source-to-solution-mapping-rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/get/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6785ACA1-B455-794D-9923-DBC2F58B25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ACC5AD-2DE8-ED41-98EA-BA2F9430042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="500" windowWidth="52940" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="146">
   <si>
     <t>shortName</t>
   </si>
@@ -344,9 +344,6 @@
     <t>Root CIM Node</t>
   </si>
   <si>
-    <t>tnt:Orphanage</t>
-  </si>
-  <si>
     <t>Orphanage</t>
   </si>
   <si>
@@ -360,12 +357,6 @@
   </si>
   <si>
     <t>Used as root asset for all CIM objects</t>
-  </si>
-  <si>
-    <t>Used to store all assets which parent does not exist</t>
-  </si>
-  <si>
-    <t>orphanage</t>
   </si>
   <si>
     <t>root-node</t>
@@ -1238,7 +1229,7 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1310,7 +1301,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2052,7 +2042,7 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="4"/>
@@ -26757,123 +26747,123 @@
       <c r="B1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="65" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="66" t="s">
+    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="66" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>139</v>
-      </c>
-    </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="53"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="51"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -26922,24 +26912,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="73"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -27103,7 +27093,7 @@
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -27262,7 +27252,7 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -27292,34 +27282,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="75" t="s">
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="74" t="s">
+      <c r="N1" s="74"/>
+      <c r="O1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -27384,37 +27374,37 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>1</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>1</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="47" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="55" t="s">
-        <v>117</v>
+      <c r="N3" s="54" t="s">
+        <v>114</v>
       </c>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
@@ -27424,37 +27414,37 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>1</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>1</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="47" t="s">
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="55" t="s">
-        <v>118</v>
+      <c r="N4" s="54" t="s">
+        <v>115</v>
       </c>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
@@ -27490,11 +27480,11 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="48" t="s">
-        <v>119</v>
+      <c r="N5" s="47" t="s">
+        <v>116</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
@@ -27530,11 +27520,11 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="N6" s="48" t="s">
-        <v>120</v>
+      <c r="N6" s="47" t="s">
+        <v>117</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
@@ -27570,11 +27560,11 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="N7" s="56" t="s">
-        <v>130</v>
+      <c r="N7" s="55" t="s">
+        <v>127</v>
       </c>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
@@ -27610,10 +27600,10 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="49" t="s">
+      <c r="N8" s="48" t="s">
         <v>95</v>
       </c>
       <c r="O8" s="17"/>
@@ -27652,11 +27642,11 @@
         <v>36</v>
       </c>
       <c r="L9" s="28"/>
-      <c r="M9" s="49" t="s">
+      <c r="M9" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="49" t="s">
-        <v>121</v>
+      <c r="N9" s="48" t="s">
+        <v>118</v>
       </c>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
@@ -27692,11 +27682,11 @@
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="50" t="s">
+      <c r="M10" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="57" t="s">
-        <v>131</v>
+      <c r="N10" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -27732,10 +27722,10 @@
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="50" t="s">
+      <c r="M11" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="N11" s="50" t="s">
+      <c r="N11" s="49" t="s">
         <v>92</v>
       </c>
       <c r="O11" s="12"/>
@@ -27774,10 +27764,10 @@
         <v>36</v>
       </c>
       <c r="L12" s="25"/>
-      <c r="M12" s="50" t="s">
+      <c r="M12" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="49" t="s">
         <v>93</v>
       </c>
       <c r="O12" s="12"/>
@@ -27816,11 +27806,11 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="58" t="s">
-        <v>132</v>
+      <c r="N13" s="57" t="s">
+        <v>129</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
@@ -27858,10 +27848,10 @@
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="40" t="s">
         <v>79</v>
       </c>
       <c r="O14" s="12"/>
@@ -27900,10 +27890,10 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="41" t="s">
+      <c r="N15" s="40" t="s">
         <v>54</v>
       </c>
       <c r="O15" s="12"/>
@@ -27940,10 +27930,10 @@
         <v>78</v>
       </c>
       <c r="L16" s="19"/>
-      <c r="M16" s="41" t="s">
+      <c r="M16" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="40" t="s">
         <v>55</v>
       </c>
       <c r="O16" s="12"/>
@@ -27980,11 +27970,11 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
-      <c r="M17" s="51" t="s">
+      <c r="M17" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="N17" s="54" t="s">
-        <v>129</v>
+      <c r="N17" s="53" t="s">
+        <v>126</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
@@ -28020,10 +28010,10 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="51" t="s">
+      <c r="M18" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="N18" s="51" t="s">
+      <c r="N18" s="50" t="s">
         <v>84</v>
       </c>
       <c r="O18" s="12"/>
@@ -28038,7 +28028,7 @@
         <v>27</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
@@ -28060,11 +28050,11 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="51" t="s">
+      <c r="M19" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="67" t="s">
-        <v>134</v>
+      <c r="N19" s="66" t="s">
+        <v>131</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -28102,11 +28092,11 @@
         <v>36</v>
       </c>
       <c r="L20" s="32"/>
-      <c r="M20" s="69" t="s">
-        <v>147</v>
-      </c>
-      <c r="N20" s="68" t="s">
-        <v>146</v>
+      <c r="M20" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="N20" s="67" t="s">
+        <v>143</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -28135,9 +28125,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8D617A-74AE-D544-8908-F3E36335854E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="233" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="233" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -28149,11 +28139,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
@@ -28167,125 +28157,70 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="39" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="37"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="40" t="s">
+      <c r="C6" s="39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="69" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>113</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>